<commit_message>
correct dates of rresearch assistant
</commit_message>
<xml_diff>
--- a/data/cv-data.xlsx
+++ b/data/cv-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8987251e2c38395f/Dokumente/Studium/cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="297" documentId="13_ncr:1_{8F600B6B-90F5-DC4B-B6D1-EA0FE5EE6490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D92DE8D-94A4-5D4E-A438-504A426B5DD3}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{8F600B6B-90F5-DC4B-B6D1-EA0FE5EE6490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA1CC91-A57C-9B44-85FD-8F698CA7D28C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
   <si>
     <t>in_resume</t>
   </si>
@@ -60,12 +60,6 @@
     <t>org</t>
   </si>
   <si>
-    <t>2014-08</t>
-  </si>
-  <si>
-    <t>2016-01</t>
-  </si>
-  <si>
     <t>award</t>
   </si>
   <si>
@@ -228,12 +222,6 @@
     <t>Undergraduate Research Assistant</t>
   </si>
   <si>
-    <t>2020-09</t>
-  </si>
-  <si>
-    <t>2019-09</t>
-  </si>
-  <si>
     <t>Took an active role in the daily care and supervision of children aged 1 to 3 years old as part of a small team</t>
   </si>
   <si>
@@ -352,6 +340,21 @@
   </si>
   <si>
     <t>expected: 04/2024</t>
+  </si>
+  <si>
+    <t>2021/08</t>
+  </si>
+  <si>
+    <t>2019/09</t>
+  </si>
+  <si>
+    <t>2020/09</t>
+  </si>
+  <si>
+    <t>2020/10</t>
+  </si>
+  <si>
+    <t>2023/03</t>
   </si>
 </sst>
 </file>
@@ -909,10 +912,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1214,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="C8:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1252,7 +1251,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s">
         <v>0</v>
@@ -1260,25 +1259,25 @@
     </row>
     <row r="2" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
         <v>59</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>61</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="J2" t="b">
         <v>1</v>
@@ -1286,25 +1285,25 @@
     </row>
     <row r="3" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -1319,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,7 +1361,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
         <v>0</v>
@@ -1370,92 +1369,95 @@
     </row>
     <row r="2" spans="1:11" ht="102" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" t="s">
         <v>66</v>
       </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="119" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" t="s">
         <v>66</v>
       </c>
-      <c r="B3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C3" t="s">
-        <v>70</v>
-      </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>109</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D4" t="s">
-        <v>56</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="H4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -1499,16 +1501,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
@@ -1517,41 +1519,41 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
-      </c>
       <c r="H2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E3">
         <v>2021</v>
@@ -1565,16 +1567,16 @@
     </row>
     <row r="4" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="D4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4">
         <v>2016</v>
@@ -1583,21 +1585,21 @@
         <v>2020</v>
       </c>
       <c r="H4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5">
         <v>2020</v>
@@ -1642,27 +1644,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2">
         <v>2022</v>
@@ -1673,10 +1675,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>2020</v>
@@ -1687,10 +1689,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>2017</v>
@@ -1701,10 +1703,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5">
         <v>2016</v>
@@ -1715,7 +1717,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -1732,10 +1734,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>2014</v>
@@ -1746,10 +1748,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>2014</v>
@@ -1760,10 +1762,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>2010</v>
@@ -1777,7 +1779,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -1794,10 +1796,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>2010</v>
@@ -1808,7 +1810,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1842,128 +1844,128 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B3">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1986,27 +1988,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update xlsx: new job
</commit_message>
<xml_diff>
--- a/data/cv-data.xlsx
+++ b/data/cv-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8987251e2c38395f/Dokumente/Studium/cv/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="13_ncr:1_{8F600B6B-90F5-DC4B-B6D1-EA0FE5EE6490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8CA1CC91-A57C-9B44-85FD-8F698CA7D28C}"/>
+  <xr:revisionPtr revIDLastSave="308" documentId="13_ncr:1_{8F600B6B-90F5-DC4B-B6D1-EA0FE5EE6490}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BE1C067-127E-B049-AAFF-797393072CAB}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="112">
   <si>
     <t>in_resume</t>
   </si>
@@ -355,6 +355,12 @@
   </si>
   <si>
     <t>2023/03</t>
+  </si>
+  <si>
+    <t>Work unit for psychological methods with interdisciplinary focus</t>
+  </si>
+  <si>
+    <t>2023/04</t>
   </si>
 </sst>
 </file>
@@ -1319,7 +1325,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1458,6 +1464,23 @@
       </c>
       <c r="K4" s="1" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>